<commit_message>
Fix Bug in CVRP_L  & Add show_function
</commit_message>
<xml_diff>
--- a/Data/HP.xlsx
+++ b/Data/HP.xlsx
@@ -463,7 +463,7 @@
         <v>47</v>
       </c>
       <c r="E4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -483,7 +483,7 @@
         <v>45</v>
       </c>
       <c r="E5">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -503,7 +503,7 @@
         <v>24</v>
       </c>
       <c r="E6">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -523,7 +523,7 @@
         <v>49</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -623,7 +623,7 @@
         <v>40</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -643,7 +643,7 @@
         <v>37</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -663,7 +663,7 @@
         <v>46</v>
       </c>
       <c r="E14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -683,7 +683,7 @@
         <v>46</v>
       </c>
       <c r="E15">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -703,7 +703,7 @@
         <v>25</v>
       </c>
       <c r="E16">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -743,7 +743,7 @@
         <v>37</v>
       </c>
       <c r="E18">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -763,7 +763,7 @@
         <v>33</v>
       </c>
       <c r="E19">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -783,7 +783,7 @@
         <v>31</v>
       </c>
       <c r="E20">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -823,7 +823,7 @@
         <v>28</v>
       </c>
       <c r="E22">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -843,7 +843,7 @@
         <v>49</v>
       </c>
       <c r="E23">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -863,7 +863,7 @@
         <v>42</v>
       </c>
       <c r="E24">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -883,7 +883,7 @@
         <v>27</v>
       </c>
       <c r="E25">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -903,7 +903,7 @@
         <v>34</v>
       </c>
       <c r="E26">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -923,7 +923,7 @@
         <v>46</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -943,7 +943,7 @@
         <v>39</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -983,7 +983,7 @@
         <v>22</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1023,7 +1023,7 @@
         <v>21</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -1043,7 +1043,7 @@
         <v>45</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -1063,7 +1063,7 @@
         <v>31</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1103,7 +1103,7 @@
         <v>44</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -1143,7 +1143,7 @@
         <v>27</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -1203,7 +1203,7 @@
         <v>39</v>
       </c>
       <c r="E41">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -1223,7 +1223,7 @@
         <v>34</v>
       </c>
       <c r="E42">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -1243,7 +1243,7 @@
         <v>49</v>
       </c>
       <c r="E43">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -1383,7 +1383,7 @@
         <v>26</v>
       </c>
       <c r="E50">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -1403,7 +1403,7 @@
         <v>31</v>
       </c>
       <c r="E51">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -1443,7 +1443,7 @@
         <v>31</v>
       </c>
       <c r="E53">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -1463,7 +1463,7 @@
         <v>37</v>
       </c>
       <c r="E54">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -1483,7 +1483,7 @@
         <v>43</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F55">
         <v>0</v>
@@ -1503,7 +1503,7 @@
         <v>27</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -1523,7 +1523,7 @@
         <v>43</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F57">
         <v>0</v>
@@ -1583,7 +1583,7 @@
         <v>26</v>
       </c>
       <c r="E60">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -1623,7 +1623,7 @@
         <v>44</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -1703,7 +1703,7 @@
         <v>25</v>
       </c>
       <c r="E66">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F66">
         <v>0</v>
@@ -1763,7 +1763,7 @@
         <v>24</v>
       </c>
       <c r="E69">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -1783,7 +1783,7 @@
         <v>46</v>
       </c>
       <c r="E70">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F70">
         <v>0</v>
@@ -1823,7 +1823,7 @@
         <v>30</v>
       </c>
       <c r="E72">
-        <v>-1</v>
+        <v>13</v>
       </c>
       <c r="F72">
         <v>0</v>
@@ -1843,7 +1843,7 @@
         <v>26</v>
       </c>
       <c r="E73">
-        <v>-1</v>
+        <v>13</v>
       </c>
       <c r="F73">
         <v>0</v>
@@ -1863,7 +1863,7 @@
         <v>42</v>
       </c>
       <c r="E74">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F74">
         <v>0</v>
@@ -1883,7 +1883,7 @@
         <v>28</v>
       </c>
       <c r="E75">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="F75">
         <v>0</v>
@@ -1903,7 +1903,7 @@
         <v>22</v>
       </c>
       <c r="E76">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F76">
         <v>0</v>
@@ -1963,7 +1963,7 @@
         <v>33</v>
       </c>
       <c r="E79">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -1983,7 +1983,7 @@
         <v>35</v>
       </c>
       <c r="E80">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F80">
         <v>0</v>
@@ -2003,7 +2003,7 @@
         <v>48</v>
       </c>
       <c r="E81">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F81">
         <v>0</v>
@@ -2023,7 +2023,7 @@
         <v>47</v>
       </c>
       <c r="E82">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F82">
         <v>0</v>
@@ -2063,7 +2063,7 @@
         <v>29</v>
       </c>
       <c r="E84">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F84">
         <v>0</v>
@@ -2083,7 +2083,7 @@
         <v>32</v>
       </c>
       <c r="E85">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F85">
         <v>0</v>
@@ -2103,7 +2103,7 @@
         <v>44</v>
       </c>
       <c r="E86">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F86">
         <v>0</v>
@@ -2123,7 +2123,7 @@
         <v>24</v>
       </c>
       <c r="E87">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F87">
         <v>0</v>
@@ -2143,7 +2143,7 @@
         <v>45</v>
       </c>
       <c r="E88">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F88">
         <v>0</v>
@@ -2163,7 +2163,7 @@
         <v>21</v>
       </c>
       <c r="E89">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F89">
         <v>0</v>
@@ -2203,7 +2203,7 @@
         <v>37</v>
       </c>
       <c r="E91">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F91">
         <v>0</v>
@@ -2223,7 +2223,7 @@
         <v>25</v>
       </c>
       <c r="E92">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F92">
         <v>0</v>
@@ -2323,7 +2323,7 @@
         <v>27</v>
       </c>
       <c r="E97">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F97">
         <v>0</v>
@@ -2343,7 +2343,7 @@
         <v>29</v>
       </c>
       <c r="E98">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F98">
         <v>0</v>
@@ -2383,7 +2383,7 @@
         <v>34</v>
       </c>
       <c r="E100">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F100">
         <v>0</v>
@@ -2403,7 +2403,7 @@
         <v>37</v>
       </c>
       <c r="E101">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F101">
         <v>0</v>
@@ -2423,7 +2423,7 @@
         <v>40</v>
       </c>
       <c r="E102">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F102">
         <v>0</v>
@@ -2443,7 +2443,7 @@
         <v>45</v>
       </c>
       <c r="E103">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F103">
         <v>0</v>
@@ -2463,7 +2463,7 @@
         <v>25</v>
       </c>
       <c r="E104">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F104">
         <v>0</v>
@@ -2483,7 +2483,7 @@
         <v>40</v>
       </c>
       <c r="E105">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F105">
         <v>0</v>
@@ -2603,7 +2603,7 @@
         <v>33</v>
       </c>
       <c r="E111">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F111">
         <v>0</v>
@@ -2663,7 +2663,7 @@
         <v>38</v>
       </c>
       <c r="E114">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F114">
         <v>0</v>
@@ -2683,7 +2683,7 @@
         <v>31</v>
       </c>
       <c r="E115">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F115">
         <v>0</v>
@@ -2703,7 +2703,7 @@
         <v>25</v>
       </c>
       <c r="E116">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F116">
         <v>0</v>
@@ -2743,7 +2743,7 @@
         <v>28</v>
       </c>
       <c r="E118">
-        <v>-1</v>
+        <v>11</v>
       </c>
       <c r="F118">
         <v>0</v>
@@ -2763,7 +2763,7 @@
         <v>25</v>
       </c>
       <c r="E119">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F119">
         <v>0</v>
@@ -2803,7 +2803,7 @@
         <v>34</v>
       </c>
       <c r="E121">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F121">
         <v>0</v>
@@ -2823,7 +2823,7 @@
         <v>25</v>
       </c>
       <c r="E122">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F122">
         <v>0</v>
@@ -2843,7 +2843,7 @@
         <v>28</v>
       </c>
       <c r="E123">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F123">
         <v>0</v>
@@ -2903,7 +2903,7 @@
         <v>23</v>
       </c>
       <c r="E126">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F126">
         <v>0</v>
@@ -2943,7 +2943,7 @@
         <v>39</v>
       </c>
       <c r="E128">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F128">
         <v>0</v>
@@ -2963,7 +2963,7 @@
         <v>35</v>
       </c>
       <c r="E129">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F129">
         <v>0</v>
@@ -2983,7 +2983,7 @@
         <v>48</v>
       </c>
       <c r="E130">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F130">
         <v>0</v>
@@ -3003,7 +3003,7 @@
         <v>39</v>
       </c>
       <c r="E131">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F131">
         <v>0</v>
@@ -3023,7 +3023,7 @@
         <v>37</v>
       </c>
       <c r="E132">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F132">
         <v>0</v>
@@ -3043,7 +3043,7 @@
         <v>28</v>
       </c>
       <c r="E133">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F133">
         <v>0</v>
@@ -3063,7 +3063,7 @@
         <v>49</v>
       </c>
       <c r="E134">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F134">
         <v>0</v>
@@ -3083,7 +3083,7 @@
         <v>25</v>
       </c>
       <c r="E135">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F135">
         <v>0</v>
@@ -3103,7 +3103,7 @@
         <v>34</v>
       </c>
       <c r="E136">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F136">
         <v>0</v>
@@ -3123,7 +3123,7 @@
         <v>40</v>
       </c>
       <c r="E137">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F137">
         <v>0</v>
@@ -3143,7 +3143,7 @@
         <v>27</v>
       </c>
       <c r="E138">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F138">
         <v>0</v>
@@ -3163,7 +3163,7 @@
         <v>26</v>
       </c>
       <c r="E139">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F139">
         <v>0</v>
@@ -3183,7 +3183,7 @@
         <v>39</v>
       </c>
       <c r="E140">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F140">
         <v>0</v>
@@ -3203,7 +3203,7 @@
         <v>45</v>
       </c>
       <c r="E141">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F141">
         <v>0</v>
@@ -3223,7 +3223,7 @@
         <v>26</v>
       </c>
       <c r="E142">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F142">
         <v>0</v>
@@ -3323,7 +3323,7 @@
         <v>45</v>
       </c>
       <c r="E147">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F147">
         <v>0</v>
@@ -3363,7 +3363,7 @@
         <v>43</v>
       </c>
       <c r="E149">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F149">
         <v>0</v>
@@ -3403,7 +3403,7 @@
         <v>33</v>
       </c>
       <c r="E151">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F151">
         <v>0</v>
@@ -3443,7 +3443,7 @@
         <v>21</v>
       </c>
       <c r="E153">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F153">
         <v>0</v>
@@ -3463,7 +3463,7 @@
         <v>39</v>
       </c>
       <c r="E154">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F154">
         <v>0</v>
@@ -3483,7 +3483,7 @@
         <v>43</v>
       </c>
       <c r="E155">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F155">
         <v>0</v>
@@ -3503,7 +3503,7 @@
         <v>46</v>
       </c>
       <c r="E156">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F156">
         <v>0</v>
@@ -3543,7 +3543,7 @@
         <v>31</v>
       </c>
       <c r="E158">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F158">
         <v>0</v>
@@ -3563,7 +3563,7 @@
         <v>34</v>
       </c>
       <c r="E159">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="F159">
         <v>0</v>
@@ -3583,7 +3583,7 @@
         <v>49</v>
       </c>
       <c r="E160">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="F160">
         <v>0</v>
@@ -3603,7 +3603,7 @@
         <v>37</v>
       </c>
       <c r="E161">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F161">
         <v>0</v>
@@ -3623,7 +3623,7 @@
         <v>28</v>
       </c>
       <c r="E162">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F162">
         <v>0</v>
@@ -3643,7 +3643,7 @@
         <v>25</v>
       </c>
       <c r="E163">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F163">
         <v>0</v>
@@ -3803,7 +3803,7 @@
         <v>39</v>
       </c>
       <c r="E171">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F171">
         <v>0</v>
@@ -3823,7 +3823,7 @@
         <v>26</v>
       </c>
       <c r="E172">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F172">
         <v>0</v>
@@ -3894,13 +3894,13 @@
         <v>174</v>
       </c>
       <c r="B176">
-        <v>1719.916974583251</v>
+        <v>1085.519200488409</v>
       </c>
       <c r="C176">
-        <v>2605.139153466509</v>
+        <v>1790.187777307487</v>
       </c>
       <c r="D176">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="E176">
         <v>0</v>
@@ -3914,13 +3914,13 @@
         <v>175</v>
       </c>
       <c r="B177">
-        <v>381.5077754268682</v>
+        <v>2347.842460310387</v>
       </c>
       <c r="C177">
-        <v>982.9680528302903</v>
+        <v>1218.924660370858</v>
       </c>
       <c r="D177">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E177">
         <v>1</v>
@@ -3934,13 +3934,13 @@
         <v>176</v>
       </c>
       <c r="B178">
-        <v>445.1968076949909</v>
+        <v>80.25953621033399</v>
       </c>
       <c r="C178">
-        <v>2518.535861883758</v>
+        <v>539.3007741857029</v>
       </c>
       <c r="D178">
-        <v>127</v>
+        <v>68</v>
       </c>
       <c r="E178">
         <v>2</v>
@@ -3954,13 +3954,13 @@
         <v>177</v>
       </c>
       <c r="B179">
-        <v>2347.842460310387</v>
+        <v>878.5546239772101</v>
       </c>
       <c r="C179">
-        <v>1218.924660370858</v>
+        <v>2525.733703979399</v>
       </c>
       <c r="D179">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="E179">
         <v>3</v>
@@ -3974,13 +3974,13 @@
         <v>178</v>
       </c>
       <c r="B180">
-        <v>1051.942866460077</v>
+        <v>2232.152399223904</v>
       </c>
       <c r="C180">
-        <v>528.8115188052595</v>
+        <v>2431.887445390206</v>
       </c>
       <c r="D180">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="E180">
         <v>4</v>
@@ -3994,13 +3994,13 @@
         <v>179</v>
       </c>
       <c r="B181">
-        <v>878.5546239772101</v>
+        <v>1051.942866460077</v>
       </c>
       <c r="C181">
-        <v>2525.733703979399</v>
+        <v>528.8115188052595</v>
       </c>
       <c r="D181">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E181">
         <v>5</v>
@@ -4014,13 +4014,13 @@
         <v>180</v>
       </c>
       <c r="B182">
-        <v>2945.464993768458</v>
+        <v>445.1968076949909</v>
       </c>
       <c r="C182">
-        <v>1351.731251727125</v>
+        <v>2518.535861883758</v>
       </c>
       <c r="D182">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="E182">
         <v>6</v>
@@ -4034,13 +4034,13 @@
         <v>181</v>
       </c>
       <c r="B183">
-        <v>1499.979726294803</v>
+        <v>2945.464993768458</v>
       </c>
       <c r="C183">
-        <v>1174.574709021907</v>
+        <v>1351.731251727125</v>
       </c>
       <c r="D183">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="E183">
         <v>7</v>
@@ -4054,10 +4054,10 @@
         <v>182</v>
       </c>
       <c r="B184">
-        <v>372.1713889649344</v>
+        <v>381.5077754268682</v>
       </c>
       <c r="C184">
-        <v>2251.16356206318</v>
+        <v>982.9680528302903</v>
       </c>
       <c r="D184">
         <v>70</v>
@@ -4074,13 +4074,13 @@
         <v>183</v>
       </c>
       <c r="B185">
-        <v>1085.519200488409</v>
+        <v>1499.979726294803</v>
       </c>
       <c r="C185">
-        <v>1790.187777307487</v>
+        <v>1174.574709021907</v>
       </c>
       <c r="D185">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="E185">
         <v>9</v>
@@ -4094,13 +4094,13 @@
         <v>184</v>
       </c>
       <c r="B186">
-        <v>2232.152399223904</v>
+        <v>1103.44024512642</v>
       </c>
       <c r="C186">
-        <v>2431.887445390206</v>
+        <v>2717.27020280983</v>
       </c>
       <c r="D186">
-        <v>72</v>
+        <v>150</v>
       </c>
       <c r="E186">
         <v>10</v>
@@ -4114,13 +4114,13 @@
         <v>185</v>
       </c>
       <c r="B187">
-        <v>80.25953621033399</v>
+        <v>636.1610031366665</v>
       </c>
       <c r="C187">
-        <v>539.3007741857029</v>
+        <v>782.3971833363092</v>
       </c>
       <c r="D187">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E187">
         <v>11</v>
@@ -4134,13 +4134,13 @@
         <v>186</v>
       </c>
       <c r="B188">
-        <v>1103.44024512642</v>
+        <v>1719.916974583251</v>
       </c>
       <c r="C188">
-        <v>2717.27020280983</v>
+        <v>2605.139153466509</v>
       </c>
       <c r="D188">
-        <v>150</v>
+        <v>41</v>
       </c>
       <c r="E188">
         <v>12</v>
@@ -4154,13 +4154,13 @@
         <v>187</v>
       </c>
       <c r="B189">
-        <v>651.5258002814537</v>
+        <v>426.4705458155561</v>
       </c>
       <c r="C189">
-        <v>621.8399603785576</v>
+        <v>2259.244686148031</v>
       </c>
       <c r="D189">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="E189">
         <v>13</v>

</xml_diff>